<commit_message>
[0300] Amended xlsx fields to use a nicer name
</commit_message>
<xml_diff>
--- a/lib/data/provider_seed_report_v_2.0_without_pii.xlsx
+++ b/lib/data/provider_seed_report_v_2.0_without_pii.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">address__address_line_1</t>
   </si>
   <si>
-    <t xml:space="preserve">address_line_2</t>
+    <t xml:space="preserve">address__address_line_2</t>
   </si>
   <si>
     <t xml:space="preserve">address__address_line_3</t>
@@ -22994,43 +22994,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -23286,8 +23286,8 @@
   </sheetPr>
   <dimension ref="A1:Q1123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A244" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F290" activeCellId="0" sqref="F290"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[0300] Import provider seed data for addresses (#323)
* [0300] Added openssl as it was causing localised issue

`SSL_connect ... certificate verify failed (unable to get certificate CRL)`

https://github.com/rails/rails/issues/55886

* [0300] Added axlsx gem

* [0300] Added write_xlsx gem

* [0300] Amended xlsx fields to use a nicer name

* [0300] Added migrations for uprn on address

Unique Property Reference Number, can be used as golden thread

* [0300] Added uprn to address from ordinance survey to model

* [0300] Removed task for address generation

* [0300] Added address cleansed rake task

* [0300] Added version bump for xlsx

* [0300] Amended helpers so it can be used with addresses

* [0300] Added uprn to address from ordinance survey to model

* [0300] Added address to be imported

* [0300] Amended helpers so it can be used with addresses

* [0300] Fixed importer for provider type school as it is absent from spreadsheet

* [0300] Removed dupe
</commit_message>
<xml_diff>
--- a/lib/data/provider_seed_report_v_2.0_without_pii.xlsx
+++ b/lib/data/provider_seed_report_v_2.0_without_pii.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">address__address_line_1</t>
   </si>
   <si>
-    <t xml:space="preserve">address_line_2</t>
+    <t xml:space="preserve">address__address_line_2</t>
   </si>
   <si>
     <t xml:space="preserve">address__address_line_3</t>
@@ -22994,43 +22994,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -23286,8 +23286,8 @@
   </sheetPr>
   <dimension ref="A1:Q1123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A244" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F290" activeCellId="0" sqref="F290"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>